<commit_message>
trying higher embedding values
</commit_message>
<xml_diff>
--- a/spreadsheets/linear_infer_testing.xlsx
+++ b/spreadsheets/linear_infer_testing.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="30">
   <si>
     <t>x</t>
   </si>
@@ -108,6 +108,15 @@
   </si>
   <si>
     <t>cbow</t>
+  </si>
+  <si>
+    <t>now try some default input: 12 +/- 15% variation</t>
+  </si>
+  <si>
+    <t>try default sticky = 10 (instead of 1), no default init</t>
+  </si>
+  <si>
+    <t>default sticky = 10</t>
   </si>
 </sst>
 </file>
@@ -2836,11 +2845,11 @@
         <v>0.48002400000000001</v>
       </c>
       <c r="N19">
-        <f t="shared" ref="N19:N26" si="2">AVERAGE(I19:M19)</f>
+        <f t="shared" ref="N19:N25" si="2">AVERAGE(I19:M19)</f>
         <v>0.48252299999999992</v>
       </c>
       <c r="O19">
-        <f t="shared" ref="O19:O26" si="3">(ABS(N19-B$7)/B$7)*100</f>
+        <f t="shared" ref="O19:O25" si="3">(ABS(N19-B$7)/B$7)*100</f>
         <v>3.4954000000000152</v>
       </c>
     </row>
@@ -3019,10 +3028,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:O61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" topLeftCell="G47" workbookViewId="0">
+      <selection activeCell="J63" sqref="J63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3059,6 +3068,9 @@
       <c r="G3" t="s">
         <v>23</v>
       </c>
+      <c r="I3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="H4" t="s">
@@ -3137,11 +3149,11 @@
         <v>10.400600000000001</v>
       </c>
       <c r="N6">
-        <f t="shared" ref="N6:N13" si="0">AVERAGE(I6:M6)</f>
+        <f t="shared" ref="N6:N12" si="0">AVERAGE(I6:M6)</f>
         <v>10.424060000000001</v>
       </c>
       <c r="O6">
-        <f t="shared" ref="O6:O13" si="1">(ABS(N6-B$7)/B$7)*100</f>
+        <f t="shared" ref="O6:O12" si="1">(ABS(N6-B$7)/B$7)*100</f>
         <v>30.506266666666658</v>
       </c>
     </row>
@@ -3381,8 +3393,11 @@
       <c r="G16" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="8:15" x14ac:dyDescent="0.3">
+      <c r="I16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="H17" t="s">
         <v>24</v>
       </c>
@@ -3408,7 +3423,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="8:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="H18">
         <v>4900</v>
       </c>
@@ -3436,7 +3451,7 @@
         <v>90.553613333333345</v>
       </c>
     </row>
-    <row r="19" spans="8:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="H19">
         <v>10000</v>
       </c>
@@ -3464,7 +3479,7 @@
         <v>86.442000000000007</v>
       </c>
     </row>
-    <row r="20" spans="8:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="H20">
         <v>100000</v>
       </c>
@@ -3492,7 +3507,7 @@
         <v>73.396333333333345</v>
       </c>
     </row>
-    <row r="21" spans="8:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="H21">
         <v>1000000</v>
       </c>
@@ -3520,44 +3535,772 @@
         <v>64.502106666666663</v>
       </c>
     </row>
-    <row r="22" spans="8:15" x14ac:dyDescent="0.3">
-      <c r="N22" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O22" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="23" spans="8:15" x14ac:dyDescent="0.3">
-      <c r="N23" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O23" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="24" spans="8:15" x14ac:dyDescent="0.3">
-      <c r="N24" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O24" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="25" spans="8:15" x14ac:dyDescent="0.3">
-      <c r="N25" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O25" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>12</v>
+      </c>
+      <c r="B26">
+        <v>0.15</v>
+      </c>
+      <c r="G26" t="s">
+        <v>23</v>
+      </c>
+      <c r="I26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H27" t="s">
+        <v>24</v>
+      </c>
+      <c r="I27" t="s">
+        <v>12</v>
+      </c>
+      <c r="J27" t="s">
+        <v>13</v>
+      </c>
+      <c r="K27" t="s">
+        <v>14</v>
+      </c>
+      <c r="L27" t="s">
+        <v>15</v>
+      </c>
+      <c r="M27" t="s">
+        <v>16</v>
+      </c>
+      <c r="N27" t="s">
+        <v>17</v>
+      </c>
+      <c r="O27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H28">
+        <v>140</v>
+      </c>
+      <c r="I28">
+        <v>13.528700000000001</v>
+      </c>
+      <c r="J28">
+        <v>13.4192</v>
+      </c>
+      <c r="K28">
+        <v>11.3794</v>
+      </c>
+      <c r="L28">
+        <v>10.9367</v>
+      </c>
+      <c r="M28">
+        <v>10.5267</v>
+      </c>
+      <c r="N28">
+        <f>AVERAGE(I28:M28)</f>
+        <v>11.95814</v>
+      </c>
+      <c r="O28">
+        <f>(ABS(N28-B$7)/B$7)*100</f>
+        <v>20.279066666666665</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H29">
+        <v>500</v>
+      </c>
+      <c r="I29">
+        <v>13.317600000000001</v>
+      </c>
+      <c r="J29">
+        <v>12.288399999999999</v>
+      </c>
+      <c r="K29">
+        <v>11.555199999999999</v>
+      </c>
+      <c r="L29">
+        <v>11.4298</v>
+      </c>
+      <c r="M29">
+        <v>13.384600000000001</v>
+      </c>
+      <c r="N29">
+        <f t="shared" ref="N29:N36" si="6">AVERAGE(I29:M29)</f>
+        <v>12.39512</v>
+      </c>
+      <c r="O29">
+        <f t="shared" ref="O29:O36" si="7">(ABS(N29-B$7)/B$7)*100</f>
+        <v>17.365866666666665</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H30">
+        <v>1000</v>
+      </c>
+      <c r="I30">
+        <v>13.328799999999999</v>
+      </c>
+      <c r="J30">
+        <v>12.9422</v>
+      </c>
+      <c r="K30">
+        <v>12.585100000000001</v>
+      </c>
+      <c r="L30">
+        <v>11.8316</v>
+      </c>
+      <c r="M30">
+        <v>13.5571</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="6"/>
+        <v>12.84896</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="7"/>
+        <v>14.340266666666668</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H31">
+        <v>5000</v>
+      </c>
+      <c r="I31">
+        <v>12.1494</v>
+      </c>
+      <c r="J31">
+        <v>11.9102</v>
+      </c>
+      <c r="K31">
+        <v>12.573</v>
+      </c>
+      <c r="L31">
+        <v>12.3009</v>
+      </c>
+      <c r="M31">
+        <v>12.1928</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="6"/>
+        <v>12.225259999999999</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="7"/>
+        <v>18.498266666666677</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H32">
+        <v>10000</v>
+      </c>
+      <c r="I32">
+        <v>11.2393</v>
+      </c>
+      <c r="J32">
+        <v>11.719200000000001</v>
+      </c>
+      <c r="K32">
+        <v>11.3957</v>
+      </c>
+      <c r="L32">
+        <v>11.2509</v>
+      </c>
+      <c r="M32">
+        <v>11.655200000000001</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="6"/>
+        <v>11.452059999999999</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="7"/>
+        <v>23.652933333333337</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H33">
+        <v>25000</v>
+      </c>
+      <c r="I33">
+        <v>9.6037999999999997</v>
+      </c>
+      <c r="J33">
+        <v>9.6806199999999993</v>
+      </c>
+      <c r="K33">
+        <v>9.5563500000000001</v>
+      </c>
+      <c r="L33">
+        <v>9.5873799999999996</v>
+      </c>
+      <c r="M33">
+        <v>9.5575899999999994</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="6"/>
+        <v>9.5971480000000007</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="7"/>
+        <v>36.019013333333326</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H34">
+        <v>750</v>
+      </c>
+      <c r="I34">
+        <v>12.2371</v>
+      </c>
+      <c r="J34">
+        <v>11.6394</v>
+      </c>
+      <c r="K34">
+        <v>13.4619</v>
+      </c>
+      <c r="L34">
+        <v>12.854200000000001</v>
+      </c>
+      <c r="M34">
+        <v>12.6899</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="6"/>
+        <v>12.576499999999999</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="7"/>
+        <v>16.156666666666673</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H35">
+        <v>900</v>
+      </c>
+      <c r="I35">
+        <v>11.682</v>
+      </c>
+      <c r="J35">
+        <v>13.4823</v>
+      </c>
+      <c r="K35">
+        <v>13.140700000000001</v>
+      </c>
+      <c r="L35">
+        <v>13.3096</v>
+      </c>
+      <c r="M35">
+        <v>12.896000000000001</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="6"/>
+        <v>12.90212</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="7"/>
+        <v>13.985866666666666</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H36">
+        <v>950</v>
+      </c>
+      <c r="I36">
+        <v>12.0997</v>
+      </c>
+      <c r="J36">
+        <v>13.8833</v>
+      </c>
+      <c r="K36">
+        <v>13.473100000000001</v>
+      </c>
+      <c r="L36">
+        <v>13.004200000000001</v>
+      </c>
+      <c r="M36">
+        <v>13.018700000000001</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="6"/>
+        <v>13.095800000000001</v>
+      </c>
+      <c r="O36">
+        <f t="shared" si="7"/>
+        <v>12.694666666666663</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G39" t="s">
+        <v>26</v>
+      </c>
+      <c r="I39" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H40" t="s">
+        <v>24</v>
+      </c>
+      <c r="I40" t="s">
+        <v>12</v>
+      </c>
+      <c r="J40" t="s">
+        <v>13</v>
+      </c>
+      <c r="K40" t="s">
+        <v>14</v>
+      </c>
+      <c r="L40" t="s">
+        <v>15</v>
+      </c>
+      <c r="M40" t="s">
+        <v>16</v>
+      </c>
+      <c r="N40" t="s">
+        <v>17</v>
+      </c>
+      <c r="O40" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H41">
+        <v>4900</v>
+      </c>
+      <c r="I41">
+        <v>1.4390400000000001</v>
+      </c>
+      <c r="J41">
+        <v>1.31037</v>
+      </c>
+      <c r="K41">
+        <v>1.33283</v>
+      </c>
+      <c r="L41">
+        <v>1.4043000000000001</v>
+      </c>
+      <c r="M41">
+        <v>1.34423</v>
+      </c>
+      <c r="N41">
+        <f>AVERAGE(I41:M41)</f>
+        <v>1.3661540000000003</v>
+      </c>
+      <c r="O41">
+        <f>(ABS(N41-B$7)/B$7)*100</f>
+        <v>90.89230666666667</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H42">
+        <v>10000</v>
+      </c>
+      <c r="I42">
+        <v>1.98106</v>
+      </c>
+      <c r="J42">
+        <v>2.0030600000000001</v>
+      </c>
+      <c r="K42">
+        <v>2.0738599999999998</v>
+      </c>
+      <c r="L42">
+        <v>1.93519</v>
+      </c>
+      <c r="M42">
+        <v>1.99722</v>
+      </c>
+      <c r="N42">
+        <f t="shared" ref="N42:N44" si="8">AVERAGE(I42:M42)</f>
+        <v>1.998078</v>
+      </c>
+      <c r="O42">
+        <f t="shared" ref="O42:O44" si="9">(ABS(N42-B$7)/B$7)*100</f>
+        <v>86.679479999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H43">
+        <v>25000</v>
+      </c>
+      <c r="I43">
+        <v>2.8906200000000002</v>
+      </c>
+      <c r="J43">
+        <v>2.8287499999999999</v>
+      </c>
+      <c r="K43">
+        <v>2.8102200000000002</v>
+      </c>
+      <c r="L43">
+        <v>2.8510300000000002</v>
+      </c>
+      <c r="M43">
+        <v>2.8502900000000002</v>
+      </c>
+      <c r="N43">
+        <f t="shared" si="8"/>
+        <v>2.8461819999999998</v>
+      </c>
+      <c r="O43">
+        <f t="shared" si="9"/>
+        <v>81.025453333333346</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H44">
+        <v>100000</v>
+      </c>
+      <c r="I44">
+        <v>3.9807600000000001</v>
+      </c>
+      <c r="J44">
+        <v>3.95892</v>
+      </c>
+      <c r="K44">
+        <v>3.9826800000000002</v>
+      </c>
+      <c r="L44">
+        <v>3.95722</v>
+      </c>
+      <c r="M44">
+        <v>3.9462700000000002</v>
+      </c>
+      <c r="N44">
+        <f t="shared" si="8"/>
+        <v>3.9651700000000005</v>
+      </c>
+      <c r="O44">
+        <f t="shared" si="9"/>
+        <v>73.565533333333335</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H45">
+        <v>250000</v>
+      </c>
+      <c r="I45">
+        <v>4.6070399999999996</v>
+      </c>
+      <c r="J45">
+        <v>4.6067400000000003</v>
+      </c>
+      <c r="K45">
+        <v>4.5976699999999999</v>
+      </c>
+      <c r="L45">
+        <v>4.5853099999999998</v>
+      </c>
+      <c r="M45">
+        <v>4.5966100000000001</v>
+      </c>
+      <c r="N45">
+        <f t="shared" ref="N45:N48" si="10">AVERAGE(I45:M45)</f>
+        <v>4.5986739999999999</v>
+      </c>
+      <c r="O45">
+        <f t="shared" ref="O45:O48" si="11">(ABS(N45-B$7)/B$7)*100</f>
+        <v>69.342173333333335</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="49" spans="7:15" x14ac:dyDescent="0.3">
+      <c r="G49" t="s">
+        <v>23</v>
+      </c>
+      <c r="I49" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="50" spans="7:15" x14ac:dyDescent="0.3">
+      <c r="H50" t="s">
+        <v>24</v>
+      </c>
+      <c r="I50" t="s">
+        <v>12</v>
+      </c>
+      <c r="J50" t="s">
+        <v>13</v>
+      </c>
+      <c r="K50" t="s">
+        <v>14</v>
+      </c>
+      <c r="L50" t="s">
+        <v>15</v>
+      </c>
+      <c r="M50" t="s">
+        <v>16</v>
+      </c>
+      <c r="N50" t="s">
+        <v>17</v>
+      </c>
+      <c r="O50" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="51" spans="7:15" x14ac:dyDescent="0.3">
+      <c r="H51">
+        <v>140</v>
+      </c>
+      <c r="I51">
+        <v>3.94842</v>
+      </c>
+      <c r="J51">
+        <v>4.2018399999999998</v>
+      </c>
+      <c r="K51">
+        <v>4.1431100000000001</v>
+      </c>
+      <c r="L51">
+        <v>4.0296500000000002</v>
+      </c>
+      <c r="M51">
+        <v>4.1268399999999996</v>
+      </c>
+      <c r="N51">
+        <f>AVERAGE(I51:M51)</f>
+        <v>4.0899720000000004</v>
+      </c>
+      <c r="O51">
+        <f>(ABS(N51-B$7)/B$7)*100</f>
+        <v>72.733520000000013</v>
+      </c>
+    </row>
+    <row r="52" spans="7:15" x14ac:dyDescent="0.3">
+      <c r="H52">
+        <v>4000</v>
+      </c>
+      <c r="I52">
+        <v>10.982100000000001</v>
+      </c>
+      <c r="J52">
+        <v>11.071199999999999</v>
+      </c>
+      <c r="K52">
+        <v>10.831099999999999</v>
+      </c>
+      <c r="L52">
+        <v>11.0284</v>
+      </c>
+      <c r="M52">
+        <v>10.8658</v>
+      </c>
+      <c r="N52">
+        <f t="shared" ref="N52:N59" si="12">AVERAGE(I52:M52)</f>
+        <v>10.955719999999999</v>
+      </c>
+      <c r="O52">
+        <f t="shared" ref="O52:O59" si="13">(ABS(N52-B$7)/B$7)*100</f>
+        <v>26.961866666666673</v>
+      </c>
+    </row>
+    <row r="53" spans="7:15" x14ac:dyDescent="0.3">
+      <c r="H53">
+        <v>10000</v>
+      </c>
+      <c r="I53">
+        <v>10.768000000000001</v>
+      </c>
+      <c r="J53">
+        <v>10.5092</v>
+      </c>
+      <c r="K53">
+        <v>10.6591</v>
+      </c>
+      <c r="L53">
+        <v>10.6387</v>
+      </c>
+      <c r="M53">
+        <v>10.5443</v>
+      </c>
+      <c r="N53">
+        <f t="shared" si="12"/>
+        <v>10.623860000000001</v>
+      </c>
+      <c r="O53">
+        <f t="shared" si="13"/>
+        <v>29.174266666666664</v>
+      </c>
+    </row>
+    <row r="54" spans="7:15" x14ac:dyDescent="0.3">
+      <c r="H54">
+        <v>6000</v>
+      </c>
+      <c r="I54">
+        <v>10.9183</v>
+      </c>
+      <c r="J54">
+        <v>11.0059</v>
+      </c>
+      <c r="K54">
+        <v>10.977399999999999</v>
+      </c>
+      <c r="L54">
+        <v>10.898199999999999</v>
+      </c>
+      <c r="M54">
+        <v>11.0359</v>
+      </c>
+      <c r="N54">
+        <f t="shared" si="12"/>
+        <v>10.967140000000001</v>
+      </c>
+      <c r="O54">
+        <f t="shared" si="13"/>
+        <v>26.885733333333327</v>
+      </c>
+    </row>
+    <row r="55" spans="7:15" x14ac:dyDescent="0.3">
+      <c r="H55">
+        <v>7000</v>
+      </c>
+      <c r="I55">
+        <v>10.7441</v>
+      </c>
+      <c r="J55">
+        <v>10.954000000000001</v>
+      </c>
+      <c r="K55">
+        <v>10.961399999999999</v>
+      </c>
+      <c r="L55">
+        <v>10.757400000000001</v>
+      </c>
+      <c r="M55">
+        <v>11.013199999999999</v>
+      </c>
+      <c r="N55">
+        <f t="shared" si="12"/>
+        <v>10.886019999999998</v>
+      </c>
+      <c r="O55">
+        <f t="shared" si="13"/>
+        <v>27.426533333333342</v>
+      </c>
+    </row>
+    <row r="57" spans="7:15" x14ac:dyDescent="0.3">
+      <c r="G57" t="s">
+        <v>26</v>
+      </c>
+      <c r="I57" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="58" spans="7:15" x14ac:dyDescent="0.3">
+      <c r="H58" t="s">
+        <v>24</v>
+      </c>
+      <c r="I58" t="s">
+        <v>12</v>
+      </c>
+      <c r="J58" t="s">
+        <v>13</v>
+      </c>
+      <c r="K58" t="s">
+        <v>14</v>
+      </c>
+      <c r="L58" t="s">
+        <v>15</v>
+      </c>
+      <c r="M58" t="s">
+        <v>16</v>
+      </c>
+      <c r="N58" t="s">
+        <v>17</v>
+      </c>
+      <c r="O58" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="59" spans="7:15" x14ac:dyDescent="0.3">
+      <c r="H59">
+        <v>4900</v>
+      </c>
+      <c r="I59">
+        <v>1.6166</v>
+      </c>
+      <c r="J59">
+        <v>1.411</v>
+      </c>
+      <c r="K59">
+        <v>1.4975000000000001</v>
+      </c>
+      <c r="L59">
+        <v>1.7015899999999999</v>
+      </c>
+      <c r="M59">
+        <v>1.4057299999999999</v>
+      </c>
+      <c r="N59">
+        <f>AVERAGE(I59:M59)</f>
+        <v>1.526484</v>
+      </c>
+      <c r="O59">
+        <f>(ABS(N59-B$7)/B$7)*100</f>
+        <v>89.823440000000005</v>
+      </c>
+    </row>
+    <row r="60" spans="7:15" x14ac:dyDescent="0.3">
+      <c r="H60">
+        <v>20000</v>
+      </c>
+      <c r="I60">
+        <v>4.1500700000000004</v>
+      </c>
+      <c r="J60">
+        <v>4.0173100000000002</v>
+      </c>
+      <c r="K60">
+        <v>4.0724600000000004</v>
+      </c>
+      <c r="L60">
+        <v>4.0721400000000001</v>
+      </c>
+      <c r="M60">
+        <v>3.9326400000000001</v>
+      </c>
+      <c r="N60">
+        <f t="shared" ref="N60:N63" si="14">AVERAGE(I60:M60)</f>
+        <v>4.0489240000000004</v>
+      </c>
+      <c r="O60">
+        <f>(ABS(N60-B$7)/B$7)*100</f>
+        <v>73.007173333333341</v>
+      </c>
+    </row>
+    <row r="61" spans="7:15" x14ac:dyDescent="0.3">
+      <c r="H61">
+        <v>100000</v>
+      </c>
+      <c r="I61">
+        <v>5.2835900000000002</v>
+      </c>
+      <c r="J61">
+        <v>5.2715300000000003</v>
+      </c>
+      <c r="K61">
+        <v>5.2834500000000002</v>
+      </c>
+      <c r="L61">
+        <v>5.2746399999999998</v>
+      </c>
+      <c r="M61">
+        <v>5.2703699999999998</v>
+      </c>
+      <c r="N61">
+        <f t="shared" si="14"/>
+        <v>5.2767160000000004</v>
+      </c>
+      <c r="O61">
+        <f>(ABS(N61-B$7)/B$7)*100</f>
+        <v>64.821893333333335</v>
       </c>
     </row>
   </sheetData>

</xml_diff>